<commit_message>
approximate costs (subject to change)
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29602"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4973AA93-C462-4F8B-867C-E842F0E670BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D2B1CA6-E8BD-431C-9006-D4FD7B29DAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,7 +117,7 @@
     <t>Hourly rate</t>
   </si>
   <si>
-    <t>Total hours</t>
+    <t>Total hours/person</t>
   </si>
   <si>
     <t>Total payout</t>
@@ -542,7 +542,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -550,7 +550,7 @@
     <col min="1" max="1" width="53" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="5" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="26.42578125" style="5" customWidth="1"/>
     <col min="6" max="6" width="118.140625" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>

</xml_diff>